<commit_message>
faltou o rafael mendes
</commit_message>
<xml_diff>
--- a/grupos-B.xlsx
+++ b/grupos-B.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="103">
   <si>
     <t>AGRO SYNC</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>CARLAO MEU PREFEITO</t>
+  </si>
+  <si>
+    <t>RAFAEL MENDES</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1075,7 @@
   <dimension ref="A2:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1083,7 @@
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -1118,7 +1121,7 @@
       <c r="B3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
         <v>74</v>
       </c>
@@ -1171,6 +1174,10 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>65</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">

</xml_diff>

<commit_message>
equipes fechadas na turma B
</commit_message>
<xml_diff>
--- a/grupos-B.xlsx
+++ b/grupos-B.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Unicesumar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Unicesumar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="B" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="109">
   <si>
     <t>AGRO SYNC</t>
   </si>
@@ -186,9 +186,6 @@
     <t>LUCAS MONTEIRO</t>
   </si>
   <si>
-    <t>SEM NOME</t>
-  </si>
-  <si>
     <t>RICARDO</t>
   </si>
   <si>
@@ -334,6 +331,27 @@
   </si>
   <si>
     <t>RAFAEL MENDES</t>
+  </si>
+  <si>
+    <t>ACERTO</t>
+  </si>
+  <si>
+    <t>VICTOR SUZUKI</t>
+  </si>
+  <si>
+    <t>VITOR COLETA</t>
+  </si>
+  <si>
+    <t>RENAN IDO</t>
+  </si>
+  <si>
+    <t>RENAN PILAN</t>
+  </si>
+  <si>
+    <t>ADEFINIDO</t>
+  </si>
+  <si>
+    <t>MATHEUS</t>
   </si>
 </sst>
 </file>
@@ -350,20 +368,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,12 +390,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -410,12 +421,12 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K34"/>
+  <dimension ref="A3:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,6 +739,15 @@
       <c r="C3" s="1">
         <v>6</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4</v>
+      </c>
       <c r="I3" s="1" t="s">
         <v>35</v>
       </c>
@@ -744,6 +764,11 @@
         <v>2</v>
       </c>
       <c r="C4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
         <v>37</v>
@@ -756,6 +781,11 @@
         <v>3</v>
       </c>
       <c r="C5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
         <v>38</v>
@@ -768,6 +798,11 @@
         <v>4</v>
       </c>
       <c r="C6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
         <v>39</v>
@@ -804,13 +839,13 @@
         <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>46</v>
@@ -830,7 +865,7 @@
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G11" s="1"/>
       <c r="I11" s="1"/>
@@ -847,7 +882,7 @@
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G12" s="1"/>
       <c r="I12" s="1"/>
@@ -864,7 +899,7 @@
       <c r="C13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G13" s="1"/>
       <c r="I13" s="1"/>
@@ -879,6 +914,11 @@
         <v>12</v>
       </c>
       <c r="C14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
         <v>45</v>
@@ -895,14 +935,14 @@
       <c r="C16" s="1">
         <v>6</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="1">
-        <v>5</v>
+      <c r="E16" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="7">
+        <v>4</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>47</v>
@@ -920,11 +960,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="1"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="7"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
         <v>49</v>
@@ -937,11 +977,11 @@
         <v>16</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="1"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" s="7"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
         <v>50</v>
@@ -954,11 +994,11 @@
         <v>17</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="1"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="7"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
         <v>51</v>
@@ -971,11 +1011,6 @@
         <v>18</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
         <v>52</v>
@@ -990,79 +1025,74 @@
       <c r="C21" s="1"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2">
-        <v>3</v>
+      <c r="C24" s="7">
+        <v>4</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="7">
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2" t="s">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2" t="s">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="2">
-        <v>3</v>
-      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="2"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1074,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,220 +1121,220 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="3"/>
+      <c r="H3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J3" s="3"/>
+      <c r="K3" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="3" t="s">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3" t="s">
-        <v>80</v>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>